<commit_message>
Added all files for Benadryl Uses
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/BenadrylUsesTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/BenadrylUsesTestData.xlsx
@@ -4,17 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12210"/>
+    <workbookView windowWidth="27945" windowHeight="12210" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="banner" sheetId="1" r:id="rId1"/>
+    <sheet name="seasonalAllergies" sheetId="2" r:id="rId2"/>
+    <sheet name="allergiesDesc" sheetId="3" r:id="rId3"/>
+    <sheet name="symptoms" sheetId="4" r:id="rId4"/>
+    <sheet name="links" sheetId="5" r:id="rId5"/>
+    <sheet name="headings" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="91">
   <si>
     <t>testcase</t>
   </si>
@@ -37,7 +42,7 @@
     <t>Verify banner content</t>
   </si>
   <si>
-    <t>yes</t>
+    <t>no</t>
   </si>
   <si>
     <t>Benadryl Difference</t>
@@ -50,6 +55,269 @@
   </si>
   <si>
     <t>BENADRYL® (diphenhydramine hydrochloride) is indicated for relief of symptoms related to hay fever, upper respiratory allergies, or cold symptoms such as:1,2</t>
+  </si>
+  <si>
+    <t>expectedHeading</t>
+  </si>
+  <si>
+    <t>expectedDescription</t>
+  </si>
+  <si>
+    <t>expectedUrl</t>
+  </si>
+  <si>
+    <t>verify 'Seasonal Allergies' heading and description. Also check 'Seasonal allergies' link.</t>
+  </si>
+  <si>
+    <t>Seasonal Allergies</t>
+  </si>
+  <si>
+    <t>Seasonal allergies are triggered by mold spores and pollens from trees, grass, and weeds. Hay fever is another name for allergic rhinitis that is caused by seasonal allergies. Depending on what you are allergic to and where you live, you may experience seasonal allergies in more than one season.3</t>
+  </si>
+  <si>
+    <t>allergies/seasonal-vs-year-round</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>Verify description for 'Pollen' under seasonal allergies</t>
+  </si>
+  <si>
+    <t>Pollen</t>
+  </si>
+  <si>
+    <t>Depending on the season and the area, trees, grasses, and weeds release pollen that can cause allergic reactions for many people. Pollen is a fine yellowish powder that is transported from plant to plant to fertilize other plants of the same species. Pollen can be transported by wind, animals, and insects.3 When breathed in, pollen can cause you to have allergy symptoms such as sneezing and a runny nose.</t>
+  </si>
+  <si>
+    <t>Verify description for 'Ragweed' under seasonal allergies</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Seasonal Allergies</t>
+    </r>
+  </si>
+  <si>
+    <t>Ragweed</t>
+  </si>
+  <si>
+    <t>Ragweed is a type of plant that can cause allergies in many people. There are 17 different types of ragweed that grow throughout the United States, and levels are higher in the late summer and fall.4</t>
+  </si>
+  <si>
+    <t>Verify description for 'Mold' under perennial allergies</t>
+  </si>
+  <si>
+    <t>Perennial Allergies</t>
+  </si>
+  <si>
+    <t>Mold</t>
+  </si>
+  <si>
+    <t>In people who have a mold allergy, being exposed to mold indoors or outdoors can cause an allergic reaction. Mold allergies can occur year-round.5</t>
+  </si>
+  <si>
+    <t>Verify description for 'Pet Dander' under perennial allergies</t>
+  </si>
+  <si>
+    <t>Pet Dander</t>
+  </si>
+  <si>
+    <t>Pet allergies are caused by an allergic reaction to proteins found in an animal's dander, saliva, or urine. Managing pet allergy symptoms can be made easier with some simple indoor allergy tips such as keeping pets off of furniture and cleaning carpets.6</t>
+  </si>
+  <si>
+    <t>Verify description for 'Dust Mites' under perennial allergies</t>
+  </si>
+  <si>
+    <t>Dust Mites</t>
+  </si>
+  <si>
+    <t>Dust mites are tiny spider-like creatures that thrive in mattresses, bedding, carpets, and upholstered furniture.7 They are a common indoor allergy trigger that can aggravate symptoms year-round.</t>
+  </si>
+  <si>
+    <t>symptom</t>
+  </si>
+  <si>
+    <t>cause</t>
+  </si>
+  <si>
+    <t>Verify decription for "Insect and Bug Bites" under itchy skin symptoms</t>
+  </si>
+  <si>
+    <t>Itchy Skin</t>
+  </si>
+  <si>
+    <t>Insect and Bug Bites</t>
+  </si>
+  <si>
+    <t>Most insect and bug bites are mild, and symptoms can be treated at home. BENADRYL® topical medicines can help relieve itching associated with insect and bug bites.8</t>
+  </si>
+  <si>
+    <t>Verify decription for "Minor Burns" under itchy skin symptoms</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14.05"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Minor Burns</t>
+    </r>
+  </si>
+  <si>
+    <t>Itching can be a symptom people experience as a minor burn heals. BENADRYL® topical medicines can help alleviate itching associated with minor burns.9</t>
+  </si>
+  <si>
+    <t>Verify decription for "Sunburn" under itchy skin symptoms</t>
+  </si>
+  <si>
+    <t>Sunburn</t>
+  </si>
+  <si>
+    <t>Sunburns can often get itchy as your skin begins to heal and scratching them can cause you even more pain. Luckily, BENADRYL® topical medicines can help alleviate itching associated with sunburns.9</t>
+  </si>
+  <si>
+    <t>Verify decription for "Minor Cuts &amp; Scrapes" under itchy skin symptoms</t>
+  </si>
+  <si>
+    <t>Minor Cuts &amp; Scrapes</t>
+  </si>
+  <si>
+    <t>Minor cuts &amp; scrapes can become itchy as they form scabs and heal. It’s important not to scratch so your wound can heal properly. BENADRYL® topical medicines can help relieve itching and pain associated with minor cuts.10</t>
+  </si>
+  <si>
+    <t>Verify decription for "Rashes Due to Poison Ivy, Poison Oak, and Poison Sumac" under itchy skin symptoms</t>
+  </si>
+  <si>
+    <t>Rashes Due to Poison Ivy, Poison Oak, and Poison Sumac</t>
+  </si>
+  <si>
+    <t>Rashes due to poisonous plants, including poison ivy, poison oak, and poison sumac can be very itchy, and they can ooze or seep discharge from of the affected skin area. BENADRYL® topical medicines can help alleviate the itching and can help dry the oozing and weeping of rashes caused by poison ivy, poison oak, and poison sumac.11</t>
+  </si>
+  <si>
+    <t>Verify decription for "Runny Nose" under itchy Cold Symptoms</t>
+  </si>
+  <si>
+    <t>Cold</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14.05"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Runny Nose</t>
+    </r>
+  </si>
+  <si>
+    <t>Runny nose is caused by mucus being discharged out of the nose with allergies or the common cold.</t>
+  </si>
+  <si>
+    <t>Verify decription for "Sneezing" under itchy Cold Symptoms</t>
+  </si>
+  <si>
+    <t>Sneezing</t>
+  </si>
+  <si>
+    <t>Sneezing can be a symptom of a cold, and it is triggered when the mucous membranes of the nose or sinuses are irritated.</t>
+  </si>
+  <si>
+    <t>Verify decription for "Congestion" under itchy Cold Symptoms</t>
+  </si>
+  <si>
+    <t>Congestion</t>
+  </si>
+  <si>
+    <t>The common cold often causes congestion of the sinuses or nasal passageways. This can happen when excess fluid causes the blood vessels and mucous membranes in the sinuses or nasal passageways to swell.</t>
+  </si>
+  <si>
+    <t>Verify decription for "Sinus Pressure" under itchy Cold Symptoms</t>
+  </si>
+  <si>
+    <t>Sinus Pressure</t>
+  </si>
+  <si>
+    <t>Sinus pressure behind the eyes and cheeks can happen when excess fluid causes the blood vessels in the mucus membrane to swell. Sinus pressure can make it difficult to breathe comfortably through the nostrils.</t>
+  </si>
+  <si>
+    <t>linktext</t>
+  </si>
+  <si>
+    <t>Verify "BENADRYL adult allergy products" link under "Which BENADRYL Product Should I Take?"</t>
+  </si>
+  <si>
+    <t>adult allergy products</t>
+  </si>
+  <si>
+    <t>products?field_product_category_tid%255B%255D=3</t>
+  </si>
+  <si>
+    <t>Verify "BENADRYL children's allergy products" link under "Which BENADRYL Product Should I Take?"</t>
+  </si>
+  <si>
+    <t>children’s allergy products</t>
+  </si>
+  <si>
+    <t>products?field_product_category_tid%255B%255D=2</t>
+  </si>
+  <si>
+    <t>Verify "BENADRYL topical products" link under "Which BENADRYL Product Should I Take?"</t>
+  </si>
+  <si>
+    <t>topical products</t>
+  </si>
+  <si>
+    <t>products?field_product_category_tid%255B%255D=4</t>
+  </si>
+  <si>
+    <t>Verify "here" link under "Which BENADRYL Product Should I Take?"</t>
+  </si>
+  <si>
+    <t>here</t>
+  </si>
+  <si>
+    <t>benadryl-dosing-guide</t>
+  </si>
+  <si>
+    <t>Verify heading "Which BENADRYL® Product Should I Take?"</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Which BENADRYL® Product Should I Take?</t>
+  </si>
+  <si>
+    <t>Verify heading "How to Use BENADRYL® Products"</t>
+  </si>
+  <si>
+    <t>How to Use BENADRYL® Products</t>
+  </si>
+  <si>
+    <t>Verify heading "BENADRYL® for Cold Symptoms"</t>
+  </si>
+  <si>
+    <t>BENADRYL® for Cold Symptoms</t>
+  </si>
+  <si>
+    <t>Verify heading "BENADRYL® for Itchy Skin Symptoms"</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>BENADRYL® for Itchy Skin Symptoms</t>
   </si>
 </sst>
 </file>
@@ -62,7 +330,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,11 +339,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -220,6 +501,13 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14.05"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="34">
@@ -531,28 +819,19 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -561,124 +840,137 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,8 +1292,8 @@
   <sheetPr/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
@@ -1011,22 +1303,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1054,4 +1346,703 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="6"/>
+  <cols>
+    <col min="6" max="6" width="19.447619047619" customWidth="1"/>
+    <col min="7" max="7" width="11.7809523809524" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <cols>
+    <col min="3" max="3" width="18.7809523809524" customWidth="1"/>
+    <col min="4" max="4" width="13.552380952381" customWidth="1"/>
+    <col min="5" max="5" width="16.8857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G5" r:id="rId1" display="Pet allergies are caused by an allergic reaction to proteins found in an animal's dander, saliva, or urine. Managing pet allergy symptoms can be made easier with some simple indoor allergy tips such as keeping pets off of furniture and cleaning carpets.6" tooltip="https://www.benadryl.com/allergies/pet-allergy-symptoms-relief"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" ht="18" spans="1:7">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" ht="18" spans="1:7">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" display="topical products" tooltip="https://www.benadryl.com/products?field_product_category_tid%5B%5D=4"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated files for Benadryl uses
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/BenadrylUsesTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/BenadrylUsesTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12210" activeTab="5"/>
+    <workbookView windowWidth="22188" windowHeight="9024" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="banner" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,16 @@
     <sheet name="symptoms" sheetId="4" r:id="rId4"/>
     <sheet name="links" sheetId="5" r:id="rId5"/>
     <sheet name="headings" sheetId="6" r:id="rId6"/>
+    <sheet name="relatedProduct" sheetId="7" r:id="rId7"/>
+    <sheet name="relatedContent" sheetId="8" r:id="rId8"/>
+    <sheet name="references" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="173">
   <si>
     <t>testcase</t>
   </si>
@@ -42,7 +45,7 @@
     <t>Verify banner content</t>
   </si>
   <si>
-    <t>no</t>
+    <t>Yes</t>
   </si>
   <si>
     <t>Benadryl Difference</t>
@@ -161,163 +164,403 @@
     <t>Verify decription for "Minor Burns" under itchy skin symptoms</t>
   </si>
   <si>
+    <t>Minor Burns</t>
+  </si>
+  <si>
+    <t>Itching can be a symptom people experience as a minor burn heals. BENADRYL® topical medicines can help alleviate itching associated with minor burns.9</t>
+  </si>
+  <si>
+    <t>Verify decription for "Sunburn" under itchy skin symptoms</t>
+  </si>
+  <si>
+    <t>Sunburn</t>
+  </si>
+  <si>
+    <t>Sunburns can often get itchy as your skin begins to heal and scratching them can cause you even more pain. Luckily, BENADRYL® topical medicines can help alleviate itching associated with sunburns.9</t>
+  </si>
+  <si>
+    <t>Verify decription for "Minor Cuts &amp; Scrapes" under itchy skin symptoms</t>
+  </si>
+  <si>
+    <t>Minor Cuts &amp; Scrapes</t>
+  </si>
+  <si>
+    <t>Minor cuts &amp; scrapes can become itchy as they form scabs and heal. It’s important not to scratch so your wound can heal properly. BENADRYL® topical medicines can help relieve itching and pain associated with minor cuts.10</t>
+  </si>
+  <si>
+    <t>Verify decription for "Rashes Due to Poison Ivy, Poison Oak, and Poison Sumac" under itchy skin symptoms</t>
+  </si>
+  <si>
+    <t>Rashes Due to Poison Ivy, Poison Oak, and Poison Sumac</t>
+  </si>
+  <si>
+    <t>Rashes due to poisonous plants, including poison ivy, poison oak, and poison sumac can be very itchy, and they can ooze or seep discharge from of the affected skin area. BENADRYL® topical medicines can help alleviate the itching and can help dry the oozing and weeping of rashes caused by poison ivy, poison oak, and poison sumac.11</t>
+  </si>
+  <si>
+    <t>Verify decription for "Runny Nose" under itchy Cold Symptoms</t>
+  </si>
+  <si>
+    <t>Cold</t>
+  </si>
+  <si>
+    <t>Runny Nose</t>
+  </si>
+  <si>
+    <t>Runny nose is caused by mucus being discharged out of the nose with allergies or the common cold.</t>
+  </si>
+  <si>
+    <t>Verify decription for "Sneezing" under itchy Cold Symptoms</t>
+  </si>
+  <si>
+    <t>Sneezing</t>
+  </si>
+  <si>
+    <t>Sneezing can be a symptom of a cold, and it is triggered when the mucous membranes of the nose or sinuses are irritated.</t>
+  </si>
+  <si>
+    <t>Verify decription for "Congestion" under itchy Cold Symptoms</t>
+  </si>
+  <si>
+    <t>Congestion</t>
+  </si>
+  <si>
+    <t>The common cold often causes congestion of the sinuses or nasal passageways. This can happen when excess fluid causes the blood vessels and mucous membranes in the sinuses or nasal passageways to swell.</t>
+  </si>
+  <si>
+    <t>Verify decription for "Sinus Pressure" under itchy Cold Symptoms</t>
+  </si>
+  <si>
+    <t>Sinus Pressure</t>
+  </si>
+  <si>
+    <t>Sinus pressure behind the eyes and cheeks can happen when excess fluid causes the blood vessels in the mucus membrane to swell. Sinus pressure can make it difficult to breathe comfortably through the nostrils.</t>
+  </si>
+  <si>
+    <t>linktext</t>
+  </si>
+  <si>
+    <t>Verify "BENADRYL adult allergy products" link under "Which BENADRYL Product Should I Take?"</t>
+  </si>
+  <si>
+    <t>adult allergy products</t>
+  </si>
+  <si>
+    <t>products?field_product_category_tid%255B%255D=3</t>
+  </si>
+  <si>
+    <t>Verify "BENADRYL children's allergy products" link under "Which BENADRYL Product Should I Take?"</t>
+  </si>
+  <si>
+    <t>children’s allergy products</t>
+  </si>
+  <si>
+    <t>products?field_product_category_tid%255B%255D=2</t>
+  </si>
+  <si>
+    <t>Verify "BENADRYL topical products" link under "Which BENADRYL Product Should I Take?"</t>
+  </si>
+  <si>
+    <t>topical products</t>
+  </si>
+  <si>
+    <t>products?field_product_category_tid%255B%255D=4</t>
+  </si>
+  <si>
+    <t>Verify "here" link under "Which BENADRYL Product Should I Take?"</t>
+  </si>
+  <si>
+    <t>here</t>
+  </si>
+  <si>
+    <t>benadryl-dosing-guide</t>
+  </si>
+  <si>
+    <t>Verify heading "Which BENADRYL® Product Should I Take?"</t>
+  </si>
+  <si>
+    <t>Which BENADRYL® Product Should I Take?</t>
+  </si>
+  <si>
+    <t>Verify heading "How to Use BENADRYL® Products"</t>
+  </si>
+  <si>
+    <t>How to Use BENADRYL® Products</t>
+  </si>
+  <si>
+    <t>Verify heading "BENADRYL® for Cold Symptoms"</t>
+  </si>
+  <si>
+    <t>BENADRYL® for Cold Symptoms</t>
+  </si>
+  <si>
+    <t>Verify heading "BENADRYL® for Itchy Skin Symptoms"</t>
+  </si>
+  <si>
+    <t>BENADRYL® for Itchy Skin Symptoms</t>
+  </si>
+  <si>
+    <t>Testcase</t>
+  </si>
+  <si>
+    <t>Execution</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>Sub Menu</t>
+  </si>
+  <si>
+    <t>Heading</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Expected URL</t>
+  </si>
+  <si>
+    <t>Ages</t>
+  </si>
+  <si>
+    <t>Product name</t>
+  </si>
+  <si>
+    <t>Verify that the header "RELATED® PRODUCTS" displayed correctly followed by the product "BENADRYL® Allergy Antihistamine Dye-Free LIQUI-GELS® with Diphenhydramine HCl 25 mg" redirecting to the correct URL, Ages and buy now button</t>
+  </si>
+  <si>
+    <t>Related Products</t>
+  </si>
+  <si>
+    <t>benadryl-allergy-dye-free-liquigels</t>
+  </si>
+  <si>
+    <t>products/benadryl-allergy-dye-free-liquigels</t>
+  </si>
+  <si>
+    <t>Ages 
+6+</t>
+  </si>
+  <si>
+    <t>Benadryl Allergy Dye-Free Liqui-Gels, 24 Count</t>
+  </si>
+  <si>
+    <t>Verify that the header "Benadryl Allergy Plus Congestion Ultratabs Tablets, 24 Count" redirecting to the correct URL, Ages and buy now button</t>
+  </si>
+  <si>
+    <t>benadryl-allergy-plus-congestion</t>
+  </si>
+  <si>
+    <t>products/benadryl-allergy-plus-congestion</t>
+  </si>
+  <si>
+    <t>Ages 
+12+</t>
+  </si>
+  <si>
+    <t>Benadryl Allergy Plus Congestion Ultratabs Tablets, 24 Count</t>
+  </si>
+  <si>
+    <t>Verify that the header "Benadryl Itch Stopping Cream, Extra Strength, 1.3 Oz
+" redirecting to the correct URL, Ages and buy now button</t>
+  </si>
+  <si>
+    <t>extra-strength-benadryl-itch-stopping-cream</t>
+  </si>
+  <si>
+    <t>products/extra-strength-benadryl-itch-stopping-cream</t>
+  </si>
+  <si>
+    <t>Ages 
+2+</t>
+  </si>
+  <si>
+    <t>Benadryl Itch Stopping Cream, Extra Strength, 1.3 Oz</t>
+  </si>
+  <si>
+    <t>Content name</t>
+  </si>
+  <si>
+    <t>Read more button</t>
+  </si>
+  <si>
+    <t>Expected Url</t>
+  </si>
+  <si>
+    <t>Check if the heading "RELATED ARTICLES" is correct and ensure that the content titled "Tips And Remedies To Treat, Prevent, And Manage Allergy Symptoms" is followed by the read more link redirecting to the correct URL</t>
+  </si>
+  <si>
+    <t>Related Articles</t>
+  </si>
+  <si>
+    <t>Tips And Remedies To Treat, Prevent, And Manage Allergy Symptoms</t>
+  </si>
+  <si>
+    <t>treatment-and-prevention</t>
+  </si>
+  <si>
+    <t>allergies/treatment-and-prevention</t>
+  </si>
+  <si>
+    <t>Check if the heading "RELATED ARTICLES" is correct and ensure that the content titled "Children’s Allergies" is followed by the read more link redirecting to the correct URL</t>
+  </si>
+  <si>
+    <t>Children’s Allergies: Common Kids Allergy Symptoms &amp; How to Help</t>
+  </si>
+  <si>
+    <t>childrens-allergies</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user is redirected to correct url after clicking on 'Cleveland Clinic. Antihistamines. July 13, 2020' link in the benadryl usage page </t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Mayo Clinic. Allergies. August 4, 2020. Accessed from</t>
+  </si>
+  <si>
+    <t>syc-20351497</t>
+  </si>
+  <si>
+    <t>https://www.mayoclinic.org/diseases-conditions/allergies/symptoms-causes/syc-20351497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user is redirected to correct url after clicking on 'Mayo Clinic. Cold or allergy: Which is it? February 17, 2022.' link in the benadryl usage page </t>
+  </si>
+  <si>
+    <t>Mayo Clinic. Cold or allergy: Which is it? February 17, 2022. Accessed from</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="14.05"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
+        <sz val="9"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Consolas"/>
         <charset val="134"/>
       </rPr>
-      <t>Minor Burns</t>
+      <t>faq-20057857</t>
     </r>
   </si>
   <si>
-    <t>Itching can be a symptom people experience as a minor burn heals. BENADRYL® topical medicines can help alleviate itching associated with minor burns.9</t>
-  </si>
-  <si>
-    <t>Verify decription for "Sunburn" under itchy skin symptoms</t>
-  </si>
-  <si>
-    <t>Sunburn</t>
-  </si>
-  <si>
-    <t>Sunburns can often get itchy as your skin begins to heal and scratching them can cause you even more pain. Luckily, BENADRYL® topical medicines can help alleviate itching associated with sunburns.9</t>
-  </si>
-  <si>
-    <t>Verify decription for "Minor Cuts &amp; Scrapes" under itchy skin symptoms</t>
-  </si>
-  <si>
-    <t>Minor Cuts &amp; Scrapes</t>
-  </si>
-  <si>
-    <t>Minor cuts &amp; scrapes can become itchy as they form scabs and heal. It’s important not to scratch so your wound can heal properly. BENADRYL® topical medicines can help relieve itching and pain associated with minor cuts.10</t>
-  </si>
-  <si>
-    <t>Verify decription for "Rashes Due to Poison Ivy, Poison Oak, and Poison Sumac" under itchy skin symptoms</t>
-  </si>
-  <si>
-    <t>Rashes Due to Poison Ivy, Poison Oak, and Poison Sumac</t>
-  </si>
-  <si>
-    <t>Rashes due to poisonous plants, including poison ivy, poison oak, and poison sumac can be very itchy, and they can ooze or seep discharge from of the affected skin area. BENADRYL® topical medicines can help alleviate the itching and can help dry the oozing and weeping of rashes caused by poison ivy, poison oak, and poison sumac.11</t>
-  </si>
-  <si>
-    <t>Verify decription for "Runny Nose" under itchy Cold Symptoms</t>
-  </si>
-  <si>
-    <t>Cold</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14.05"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Runny Nose</t>
-    </r>
-  </si>
-  <si>
-    <t>Runny nose is caused by mucus being discharged out of the nose with allergies or the common cold.</t>
-  </si>
-  <si>
-    <t>Verify decription for "Sneezing" under itchy Cold Symptoms</t>
-  </si>
-  <si>
-    <t>Sneezing</t>
-  </si>
-  <si>
-    <t>Sneezing can be a symptom of a cold, and it is triggered when the mucous membranes of the nose or sinuses are irritated.</t>
-  </si>
-  <si>
-    <t>Verify decription for "Congestion" under itchy Cold Symptoms</t>
-  </si>
-  <si>
-    <t>Congestion</t>
-  </si>
-  <si>
-    <t>The common cold often causes congestion of the sinuses or nasal passageways. This can happen when excess fluid causes the blood vessels and mucous membranes in the sinuses or nasal passageways to swell.</t>
-  </si>
-  <si>
-    <t>Verify decription for "Sinus Pressure" under itchy Cold Symptoms</t>
-  </si>
-  <si>
-    <t>Sinus Pressure</t>
-  </si>
-  <si>
-    <t>Sinus pressure behind the eyes and cheeks can happen when excess fluid causes the blood vessels in the mucus membrane to swell. Sinus pressure can make it difficult to breathe comfortably through the nostrils.</t>
-  </si>
-  <si>
-    <t>linktext</t>
-  </si>
-  <si>
-    <t>Verify "BENADRYL adult allergy products" link under "Which BENADRYL Product Should I Take?"</t>
-  </si>
-  <si>
-    <t>adult allergy products</t>
-  </si>
-  <si>
-    <t>products?field_product_category_tid%255B%255D=3</t>
-  </si>
-  <si>
-    <t>Verify "BENADRYL children's allergy products" link under "Which BENADRYL Product Should I Take?"</t>
-  </si>
-  <si>
-    <t>children’s allergy products</t>
-  </si>
-  <si>
-    <t>products?field_product_category_tid%255B%255D=2</t>
-  </si>
-  <si>
-    <t>Verify "BENADRYL topical products" link under "Which BENADRYL Product Should I Take?"</t>
-  </si>
-  <si>
-    <t>topical products</t>
-  </si>
-  <si>
-    <t>products?field_product_category_tid%255B%255D=4</t>
-  </si>
-  <si>
-    <t>Verify "here" link under "Which BENADRYL Product Should I Take?"</t>
-  </si>
-  <si>
-    <t>here</t>
-  </si>
-  <si>
-    <t>benadryl-dosing-guide</t>
-  </si>
-  <si>
-    <t>Verify heading "Which BENADRYL® Product Should I Take?"</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Which BENADRYL® Product Should I Take?</t>
-  </si>
-  <si>
-    <t>Verify heading "How to Use BENADRYL® Products"</t>
-  </si>
-  <si>
-    <t>How to Use BENADRYL® Products</t>
-  </si>
-  <si>
-    <t>Verify heading "BENADRYL® for Cold Symptoms"</t>
-  </si>
-  <si>
-    <t>BENADRYL® for Cold Symptoms</t>
-  </si>
-  <si>
-    <t>Verify heading "BENADRYL® for Itchy Skin Symptoms"</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>BENADRYL® for Itchy Skin Symptoms</t>
+    <t>https://www.mayoclinic.org/diseases-conditions/common-cold/expert-answers/common-cold/faq-20057857</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user is redirected to correct url after clicking on 'Mayo Clinic. Seasonal allergies: Nip them in the bud. April 16, 2020' link in the benadryl usage page </t>
+  </si>
+  <si>
+    <t>Mayo Clinic. Seasonal allergies: Nip them in the bud. April 16, 2020. Accessed from</t>
+  </si>
+  <si>
+    <t>art-20048343</t>
+  </si>
+  <si>
+    <t>https://www.mayoclinic.org/diseases-conditions/hay-fever/in-depth/seasonal-allergies/art-20048343</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user is redirected to correct url after clicking on 'American College of Asthma, Allergy, and Immunology. Ragweed Allergy. April 23, 2018' link in the benadryl usage page </t>
+  </si>
+  <si>
+    <t>American College of Asthma, Allergy, and Immunology. Ragweed Allergy. April 23, 2018. Accessed from</t>
+  </si>
+  <si>
+    <t>allergic-conditions/ragweed-allergy</t>
+  </si>
+  <si>
+    <t>https://acaai.org/allergies/allergic-conditions/ragweed-allergy/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user is redirected to correct url after clicking on 'Mayo Clinic. Mold allergy. June 21, 2021' link in the benadryl usage page </t>
+  </si>
+  <si>
+    <t>Mayo Clinic. Mold allergy. June 21, 2021. Accessed from</t>
+  </si>
+  <si>
+    <t>syc-20351519</t>
+  </si>
+  <si>
+    <t>https://www.mayoclinic.org/diseases-conditions/mold-allergy/symptoms-causes/syc-20351519</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user is redirected to correct url after clicking on 'Mayo Clinic. Pet allergy. August 4, 2021' link in the benadryl usage page </t>
+  </si>
+  <si>
+    <t>Mayo Clinic. Pet allergy. August 4, 2021. Accessed from</t>
+  </si>
+  <si>
+    <t>syc-20352192</t>
+  </si>
+  <si>
+    <t>https://www.mayoclinic.org/diseases-conditions/pet-allergy/symptoms-causes/syc-20352192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user is redirected to correct url after clicking on 'Asthma and Allergy Foundation of America. Dust Mite Allergy. October 2015' link in the benadryl usage page </t>
+  </si>
+  <si>
+    <t>Asthma and Allergy Foundation of America. Dust Mite Allergy. October 2015</t>
+  </si>
+  <si>
+    <t>dust-mite-allergy</t>
+  </si>
+  <si>
+    <t>https://aafa.org/allergies/types-of-allergies/insect-allergy/dust-mite-allergy/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user is redirected to correct url after clicking on 'American Acacemy of Dermatology Association. Tips to prevent and treat bug bites' link in the benadryl usage page </t>
+  </si>
+  <si>
+    <t>American Acacemy of Dermatology Association. Tips to prevent and treat bug bites</t>
+  </si>
+  <si>
+    <t>bites/prevent-treat-bug-bites</t>
+  </si>
+  <si>
+    <t>https://www.aad.org/public/everyday-care/injured-skin/bites/prevent-treat-bug-bites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user is redirected to correct url after clicking on 'UpToDate. Patient education: Skin burns (Beyond the Basics). July 26, 2021.' link in the benadryl usage page </t>
+  </si>
+  <si>
+    <t>UpToDate. Patient education: Skin burns (Beyond the Basics). July 26, 2021</t>
+  </si>
+  <si>
+    <t>skin-burns-beyond-the-basics/print</t>
+  </si>
+  <si>
+    <t>https://www.uptodate.com/contents/skin-burns-beyond-the-basics/print?source=outline_link&amp;view=text&amp;anchor=H14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user is redirected to correct url after clicking on 'Mayo Clinic. Cuts and scrapes: First aid. November 17, 2021' link in the benadryl usage page </t>
+  </si>
+  <si>
+    <t>Mayo Clinic. Cuts and scrapes: First aid. November 17, 2021</t>
+  </si>
+  <si>
+    <t>art-20056711</t>
+  </si>
+  <si>
+    <t>https://www.mayoclinic.org/first-aid/first-aid-cuts/basics/art-20056711</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user is redirected to correct url after clicking on 'Cleveland Clinic. Poison Ivy, Poison Oak and Poison Sumac. August 4, 2020' link in the benadryl usage page </t>
+  </si>
+  <si>
+    <t>Cleveland Clinic. Poison Ivy, Poison Oak and Poison Sumac. August 4, 2020</t>
+  </si>
+  <si>
+    <t>poison-oak--poison-sumac</t>
+  </si>
+  <si>
+    <t>https://my.clevelandclinic.org/health/diseases/10655-poison-plants-poison-ivy--poison-oak--poison-sumac</t>
   </si>
 </sst>
 </file>
@@ -330,7 +573,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,10 +590,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
@@ -359,11 +604,28 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -502,20 +764,19 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14.05"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -834,143 +1095,178 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1296,29 +1592,29 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
   <cols>
-    <col min="5" max="5" width="92.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="158.285714285714" customWidth="1"/>
+    <col min="5" max="5" width="92.5740740740741" customWidth="1"/>
+    <col min="6" max="6" width="158.287037037037" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1354,35 +1650,35 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="6" max="6" width="19.447619047619" customWidth="1"/>
-    <col min="7" max="7" width="11.7809523809524" customWidth="1"/>
+    <col min="6" max="6" width="19.4444444444444" customWidth="1"/>
+    <col min="7" max="7" width="11.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1420,37 +1716,37 @@
   <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="3" max="3" width="18.7809523809524" customWidth="1"/>
-    <col min="4" max="4" width="13.552380952381" customWidth="1"/>
-    <col min="5" max="5" width="16.8857142857143" customWidth="1"/>
+    <col min="3" max="3" width="18.7777777777778" customWidth="1"/>
+    <col min="4" max="4" width="13.5555555555556" customWidth="1"/>
+    <col min="5" max="5" width="16.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1490,7 +1786,7 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="21" t="s">
         <v>24</v>
       </c>
       <c r="F3" t="s">
@@ -1584,31 +1880,31 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="B9" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1635,7 +1931,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" ht="18" spans="1:7">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1651,7 +1947,7 @@
       <c r="E3" t="s">
         <v>40</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="19" t="s">
         <v>44</v>
       </c>
       <c r="G3" t="s">
@@ -1727,7 +2023,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" ht="18" spans="1:7">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1743,10 +2039,10 @@
       <c r="E7" t="s">
         <v>56</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="19" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1831,28 +2127,28 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1889,7 +2185,7 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>73</v>
       </c>
       <c r="F3" t="s">
@@ -1950,26 +2246,26 @@
   <sheetPr/>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="4"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1977,72 +2273,646 @@
       <c r="A2" t="s">
         <v>81</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>82</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>84</v>
-      </c>
-      <c r="B3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>86</v>
-      </c>
-      <c r="B4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
         <v>88</v>
-      </c>
-      <c r="B5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="3"/>
+  <cols>
+    <col min="1" max="1" width="45.1388888888889" customWidth="1"/>
+    <col min="6" max="6" width="42.287037037037" customWidth="1"/>
+    <col min="7" max="7" width="45.287037037037" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="21" customHeight="1" spans="1:9">
+      <c r="A1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" ht="21" customHeight="1" spans="1:9">
+      <c r="A2" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" ht="21" customHeight="1" spans="1:9">
+      <c r="A3" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" ht="28.8" spans="1:9">
+      <c r="A4" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" ht="31" customHeight="1" spans="1:8">
+      <c r="A2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" ht="31" customHeight="1" spans="1:8">
+      <c r="A3" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="5" width="9.13888888888889" style="2"/>
+    <col min="6" max="6" width="48.5740740740741" style="2" customWidth="1"/>
+    <col min="7" max="8" width="9.13888888888889" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:8">
+      <c r="A1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" ht="27" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="https://www.mayoclinic.org/diseases-conditions/allergies/symptoms-causes/syc-20351497"/>
+    <hyperlink ref="H3" r:id="rId2" display="https://www.mayoclinic.org/diseases-conditions/common-cold/expert-answers/common-cold/faq-20057857"/>
+    <hyperlink ref="H4" r:id="rId3" display="https://www.mayoclinic.org/diseases-conditions/hay-fever/in-depth/seasonal-allergies/art-20048343"/>
+    <hyperlink ref="H6" r:id="rId4" display="https://www.mayoclinic.org/diseases-conditions/mold-allergy/symptoms-causes/syc-20351519"/>
+    <hyperlink ref="H11" r:id="rId5" display="https://www.mayoclinic.org/first-aid/first-aid-cuts/basics/art-20056711"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>